<commit_message>
qti batch 3 updates
</commit_message>
<xml_diff>
--- a/documents/SB_QTI_ExampleItems_Batch3.xlsx
+++ b/documents/SB_QTI_ExampleItems_Batch3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20370"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\smarterapp.github.io\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rachelkachchaf/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4FDFB03-763B-43D3-A205-D001AEBB2F66}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B54DEF8-4CC4-F144-B6DE-A67C7D38A182}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="11325" xr2:uid="{6AB3468F-8B3B-2144-B7FE-C009B0FBBD36}"/>
+    <workbookView xWindow="12480" yWindow="2180" windowWidth="18980" windowHeight="16860" xr2:uid="{6AB3468F-8B3B-2144-B7FE-C009B0FBBD36}"/>
   </bookViews>
   <sheets>
     <sheet name="QTI Sample Master List" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="50">
   <si>
     <t>Type </t>
   </si>
@@ -57,9 +57,6 @@
     <t>TTS </t>
   </si>
   <si>
-    <t>TTSVI </t>
-  </si>
-  <si>
     <t>Image </t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>n/a</t>
-  </si>
-  <si>
     <t>MC</t>
   </si>
   <si>
@@ -144,9 +138,6 @@
     <t xml:space="preserve">183685	</t>
   </si>
   <si>
-    <t xml:space="preserve">182938	</t>
-  </si>
-  <si>
     <t xml:space="preserve">183197	</t>
   </si>
   <si>
@@ -168,9 +159,6 @@
     <t xml:space="preserve">183093	</t>
   </si>
   <si>
-    <t xml:space="preserve">182865	</t>
-  </si>
-  <si>
     <t xml:space="preserve">183477	</t>
   </si>
   <si>
@@ -184,6 +172,9 @@
   </si>
   <si>
     <t xml:space="preserve">182951	</t>
+  </si>
+  <si>
+    <t>Spanish TTS</t>
   </si>
 </sst>
 </file>
@@ -592,28 +583,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7E10AB2-B4E9-4A43-A457-07B9F0A22470}">
-  <dimension ref="A1:V18"/>
+  <dimension ref="A1:V16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.375" style="5" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" style="5" customWidth="1"/>
     <col min="2" max="2" width="17" style="5" customWidth="1"/>
-    <col min="3" max="4" width="9.375" style="5" customWidth="1"/>
+    <col min="3" max="4" width="9.33203125" style="5" customWidth="1"/>
     <col min="5" max="5" width="6" style="5" customWidth="1"/>
-    <col min="6" max="6" width="5.125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="5.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" style="5" customWidth="1"/>
     <col min="8" max="8" width="4" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="3.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="3.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.5" style="5" customWidth="1"/>
+    <col min="12" max="12" width="3.5" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="4" style="5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="3.5" style="5" bestFit="1" customWidth="1"/>
     <col min="16" max="22" width="4" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" s="1" customFormat="1" ht="60" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -645,183 +638,183 @@
         <v>9</v>
       </c>
       <c r="K1" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="N1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="O1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="P1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="Q1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="R1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="S1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="T1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="11" t="s">
+      <c r="U1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="V1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="11" t="s">
+    </row>
+    <row r="2" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>22</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5">
         <v>3</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G2" s="5">
         <v>1</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="O2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="R2" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="S2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="T2" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="V2" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="B3" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5">
         <v>3</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G3" s="5">
         <v>1</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="P3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="R3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="S3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="T3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="U3" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="V3" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>27</v>
-      </c>
       <c r="B4" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D4" s="5">
         <v>193799</v>
@@ -830,565 +823,855 @@
         <v>3</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G4" s="5">
         <v>3</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q4" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="R4" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S4" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="T4" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="U4" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="V4" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E5" s="5">
         <v>3</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G5" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="S5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="T5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="U5" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="V5" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E6" s="5">
         <v>3</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G6" s="5">
-        <v>4</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>24</v>
+        <v>1</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="R6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="S6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="T6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="U6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="V6" s="6" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
+      </c>
+      <c r="D7" s="5">
+        <v>193792</v>
       </c>
       <c r="E7" s="5">
         <v>3</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G7" s="5">
         <v>1</v>
       </c>
-      <c r="H7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="8" t="s">
+      <c r="H7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="R7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="S7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="T7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="U7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="V7" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="J7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="L7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="M7" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="N7" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="O7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="P7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="R7" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="S7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="T7" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="U7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="V7" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="B8" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D8" s="5">
-        <v>193792</v>
+        <v>193799</v>
       </c>
       <c r="E8" s="5">
         <v>3</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G8" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="R8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="S8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="T8" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="U8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="V8" s="8" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>22</v>
+        <v>32</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="5">
-        <v>193799</v>
+        <v>41</v>
       </c>
       <c r="E9" s="5">
         <v>3</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G9" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="R9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="T9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="U9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="V9" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="J9" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="P9" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q9" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="R9" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="S9" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="T9" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="U9" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="V9" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="B10" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E10" s="5">
         <v>3</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G10" s="5">
         <v>2</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="S10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="T10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="U10" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="V10" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>22</v>
+        <v>33</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>21</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E11" s="5">
         <v>3</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G11" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="R11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="T11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="U11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="V11" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E12" s="5">
         <v>3</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G12" s="5">
         <v>1</v>
       </c>
-      <c r="H12" s="5" t="s">
-        <v>24</v>
+      <c r="H12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="P12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="R12" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="T12" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="U12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="V12" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+      <c r="D13" s="5">
+        <v>193792</v>
       </c>
       <c r="E13" s="5">
         <v>3</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G13" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>24</v>
       </c>
+      <c r="I13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="R13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="T13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="U13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="V13" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="D14" s="5">
+        <v>193799</v>
       </c>
       <c r="E14" s="5">
         <v>3</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G14" s="5">
-        <v>1</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="L14" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="M14" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M14" s="8" t="s">
         <v>24</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="O14" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="P14" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="P14" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="Q14" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="R14" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="S14" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="T14" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="U14" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="V14" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
+      </c>
+      <c r="R14" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="S14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="T14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="U14" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="V14" s="8" t="s">
+        <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="5">
-        <v>193792</v>
+        <v>47</v>
       </c>
       <c r="E15" s="5">
         <v>3</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G15" s="5">
         <v>1</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="R15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="T15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="U15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="V15" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="5">
-        <v>193799</v>
+        <v>48</v>
       </c>
       <c r="E16" s="5">
         <v>3</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G16" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="J16" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="K16" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="L16" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="M16" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="N16" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="O16" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="P16" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q16" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="R16" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="S16" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="T16" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="U16" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="V16" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="5">
-        <v>3</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="G17" s="5">
-        <v>1</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="E18" s="5">
-        <v>3</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G18" s="5">
-        <v>2</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="M16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="R16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="T16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="U16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="V16" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B62:B65" xr:uid="{8864DD3F-8E4E-4822-8101-94BB6DA6B810}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B60:B63" xr:uid="{8864DD3F-8E4E-4822-8101-94BB6DA6B810}">
       <formula1>"Selected, QC in progress, Pending, Ready for Release"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B28:B61 B2:B18" xr:uid="{5B37AC3B-1C04-4106-8720-CD60A5E962F6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B26:B59 B2:B16" xr:uid="{5B37AC3B-1C04-4106-8720-CD60A5E962F6}">
       <formula1>"Selected, QC in progress, Pending, Fail, Ready for Release"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1397,6 +1680,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MigrationWizId xmlns="15a21681-0ca0-46d2-8858-25ef113211f0" xsi:nil="true"/>
+    <MigrationWizIdSecurityGroups xmlns="15a21681-0ca0-46d2-8858-25ef113211f0" xsi:nil="true"/>
+    <MigrationWizIdDocumentLibraryPermissions xmlns="15a21681-0ca0-46d2-8858-25ef113211f0" xsi:nil="true"/>
+    <MigrationWizIdPermissionLevels xmlns="15a21681-0ca0-46d2-8858-25ef113211f0" xsi:nil="true"/>
+    <MigrationWizIdPermissions xmlns="15a21681-0ca0-46d2-8858-25ef113211f0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100988D3A5DB1F2074D91EDDD82E1316EE7" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b397e7678ea470e0219e6f076e5413cb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="15a21681-0ca0-46d2-8858-25ef113211f0" xmlns:ns3="e556f37e-2269-4362-849b-5bffb61b521a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a3621bbc41f10ec74d9da89ab8237e05" ns2:_="" ns3:_="">
     <xsd:import namespace="15a21681-0ca0-46d2-8858-25ef113211f0"/>
@@ -1637,42 +1941,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MigrationWizId xmlns="15a21681-0ca0-46d2-8858-25ef113211f0" xsi:nil="true"/>
-    <MigrationWizIdSecurityGroups xmlns="15a21681-0ca0-46d2-8858-25ef113211f0" xsi:nil="true"/>
-    <MigrationWizIdDocumentLibraryPermissions xmlns="15a21681-0ca0-46d2-8858-25ef113211f0" xsi:nil="true"/>
-    <MigrationWizIdPermissionLevels xmlns="15a21681-0ca0-46d2-8858-25ef113211f0" xsi:nil="true"/>
-    <MigrationWizIdPermissions xmlns="15a21681-0ca0-46d2-8858-25ef113211f0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22580FCF-5F76-4E85-89AD-ECCD571F4D4C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7847A3B2-3DDC-4291-8669-871C9CD1CAD5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="15a21681-0ca0-46d2-8858-25ef113211f0"/>
-    <ds:schemaRef ds:uri="e556f37e-2269-4362-849b-5bffb61b521a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1695,9 +1967,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7847A3B2-3DDC-4291-8669-871C9CD1CAD5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{22580FCF-5F76-4E85-89AD-ECCD571F4D4C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="15a21681-0ca0-46d2-8858-25ef113211f0"/>
+    <ds:schemaRef ds:uri="e556f37e-2269-4362-849b-5bffb61b521a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>